<commit_message>
this is it, i'm done
</commit_message>
<xml_diff>
--- a/ExperimentalData.xlsx
+++ b/ExperimentalData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rick\Documents\cs170\project1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E55B1D0-0563-40C9-B61E-BE90D937E34F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D869C48-0B97-420E-AE58-460ACFC5CA29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{9E63FDFC-2A19-4150-9F40-25391B7663C4}"/>
+    <workbookView xWindow="-30828" yWindow="-6240" windowWidth="30936" windowHeight="18696" activeTab="3" xr2:uid="{9E63FDFC-2A19-4150-9F40-25391B7663C4}"/>
   </bookViews>
   <sheets>
     <sheet name="CheckRepeated" sheetId="1" r:id="rId1"/>
@@ -2846,22 +2846,22 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>233</c:v>
+                  <c:v>309</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1904</c:v>
+                  <c:v>2239</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14570</c:v>
+                  <c:v>14190</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>42262</c:v>
+                  <c:v>41909</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>126795</c:v>
+                  <c:v>134336</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2963,16 +2963,16 @@
                   <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>96</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>627</c:v>
+                  <c:v>666</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2772</c:v>
+                  <c:v>3146</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>14168</c:v>
+                  <c:v>17769</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3077,13 +3077,13 @@
                   <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>91</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>236</c:v>
+                  <c:v>503</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1391</c:v>
+                  <c:v>1758</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3389,6 +3389,7 @@
         <c:axId val="786108192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="140000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3712,25 +3713,25 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>37</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>253</c:v>
+                  <c:v>188</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2018</c:v>
+                  <c:v>1268</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13429</c:v>
+                  <c:v>6739</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>35026</c:v>
+                  <c:v>17612</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>63230</c:v>
+                  <c:v>24203</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3823,25 +3824,25 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>33</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>113</c:v>
+                  <c:v>84</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>648</c:v>
+                  <c:v>414</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2892</c:v>
+                  <c:v>1831</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>13328</c:v>
+                  <c:v>8717</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3934,25 +3935,25 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>98</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>257</c:v>
+                  <c:v>306</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1455</c:v>
+                  <c:v>967</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4588,16 +4589,16 @@
                   <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>120</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>424</c:v>
+                  <c:v>338</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1518</c:v>
+                  <c:v>1143</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2502</c:v>
+                  <c:v>1540</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4708,13 +4709,13 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>123</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1531</c:v>
+                  <c:v>1230</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4825,13 +4826,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>100</c:v>
+                  <c:v>140</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5079,7 +5080,6 @@
         <c:axId val="483135279"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="3000"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -8657,12 +8657,12 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.81195</cdr:x>
-      <cdr:y>0.81248</cdr:y>
+      <cdr:x>0.80653</cdr:x>
+      <cdr:y>0.77245</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.97466</cdr:x>
-      <cdr:y>0.86252</cdr:y>
+      <cdr:x>0.96924</cdr:x>
+      <cdr:y>0.82249</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -8677,8 +8677,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="7985125" y="4794250"/>
-          <a:ext cx="1600200" cy="295275"/>
+          <a:off x="7930287" y="4558012"/>
+          <a:ext cx="1599871" cy="295273"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -8766,12 +8766,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.81872</cdr:x>
-      <cdr:y>0.39118</cdr:y>
+      <cdr:x>0.8071</cdr:x>
+      <cdr:y>0.2982</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.99693</cdr:x>
-      <cdr:y>0.45736</cdr:y>
+      <cdr:x>0.98531</cdr:x>
+      <cdr:y>0.36438</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -8786,8 +8786,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="8051800" y="2308225"/>
-          <a:ext cx="1752600" cy="390525"/>
+          <a:off x="7935894" y="1759611"/>
+          <a:ext cx="1752278" cy="390511"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -8862,7 +8862,7 @@
         </a:lstStyle>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
-            <a:rPr lang="en-US" sz="1200">
+            <a:rPr lang="en-US" sz="1100">
               <a:solidFill>
                 <a:schemeClr val="bg2">
                   <a:lumMod val="50000"/>
@@ -8872,7 +8872,7 @@
             <a:t>A*</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" sz="1200" baseline="0">
+            <a:rPr lang="en-US" sz="1100" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="bg2">
                   <a:lumMod val="50000"/>
@@ -8881,7 +8881,7 @@
             </a:rPr>
             <a:t> Misplaced Tiles</a:t>
           </a:r>
-          <a:endParaRPr lang="en-US" sz="1200">
+          <a:endParaRPr lang="en-US" sz="1100">
             <a:solidFill>
               <a:schemeClr val="bg2">
                 <a:lumMod val="50000"/>
@@ -8894,12 +8894,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.81098</cdr:x>
-      <cdr:y>0.17003</cdr:y>
+      <cdr:x>0.77688</cdr:x>
+      <cdr:y>0.15453</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.96005</cdr:x>
-      <cdr:y>0.24953</cdr:y>
+      <cdr:x>0.92595</cdr:x>
+      <cdr:y>0.23403</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -8914,8 +8914,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="7975600" y="1003300"/>
-          <a:ext cx="1466055" cy="469107"/>
+          <a:off x="7638809" y="911862"/>
+          <a:ext cx="1465754" cy="469109"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -8990,7 +8990,7 @@
         </a:lstStyle>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
-            <a:rPr lang="en-US" sz="1200">
+            <a:rPr lang="en-US" sz="1100">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -9995,12 +9995,12 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.797</cdr:x>
-      <cdr:y>0.12029</cdr:y>
+      <cdr:x>0.7911</cdr:x>
+      <cdr:y>0.11414</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.93897</cdr:x>
-      <cdr:y>0.196</cdr:y>
+      <cdr:x>0.93307</cdr:x>
+      <cdr:y>0.18985</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -10015,8 +10015,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="8230394" y="745332"/>
-          <a:ext cx="1466055" cy="469107"/>
+          <a:off x="8169412" y="707448"/>
+          <a:ext cx="1466080" cy="469244"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -10027,7 +10027,7 @@
         <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
-            <a:rPr lang="en-US" sz="1200">
+            <a:rPr lang="en-US" sz="1100">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -10040,12 +10040,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.79231</cdr:x>
-      <cdr:y>0.71407</cdr:y>
+      <cdr:x>0.71188</cdr:x>
+      <cdr:y>0.76694</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.96203</cdr:x>
-      <cdr:y>0.77709</cdr:y>
+      <cdr:x>0.8816</cdr:x>
+      <cdr:y>0.82996</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -10060,8 +10060,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="8181975" y="4424364"/>
-          <a:ext cx="1752600" cy="390525"/>
+          <a:off x="7351360" y="4753408"/>
+          <a:ext cx="1752646" cy="390593"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -10072,7 +10072,7 @@
         <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
-            <a:rPr lang="en-US" sz="1200">
+            <a:rPr lang="en-US" sz="1100">
               <a:solidFill>
                 <a:schemeClr val="bg2">
                   <a:lumMod val="50000"/>
@@ -10082,7 +10082,7 @@
             <a:t>A*</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" sz="1200" baseline="0">
+            <a:rPr lang="en-US" sz="1100" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="bg2">
                   <a:lumMod val="50000"/>
@@ -10091,7 +10091,7 @@
             </a:rPr>
             <a:t> Misplaced Tiles</a:t>
           </a:r>
-          <a:endParaRPr lang="en-US" sz="1200">
+          <a:endParaRPr lang="en-US" sz="1100">
             <a:solidFill>
               <a:schemeClr val="bg2">
                 <a:lumMod val="50000"/>
@@ -10156,12 +10156,12 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.78183</cdr:x>
-      <cdr:y>0.10521</cdr:y>
+      <cdr:x>0.72346</cdr:x>
+      <cdr:y>0.18522</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.92402</cdr:x>
-      <cdr:y>0.16089</cdr:y>
+      <cdr:x>0.86565</cdr:x>
+      <cdr:y>0.2409</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -10176,8 +10176,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="8061325" y="650876"/>
-          <a:ext cx="1466055" cy="344490"/>
+          <a:off x="7460813" y="1146581"/>
+          <a:ext cx="1466366" cy="344676"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -10252,7 +10252,7 @@
         </a:lstStyle>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
-            <a:rPr lang="en-US" sz="1200">
+            <a:rPr lang="en-US" sz="1100">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -10265,12 +10265,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.78922</cdr:x>
-      <cdr:y>0.60405</cdr:y>
+      <cdr:x>0.75449</cdr:x>
+      <cdr:y>0.6139</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.9592</cdr:x>
-      <cdr:y>0.66718</cdr:y>
+      <cdr:x>0.92447</cdr:x>
+      <cdr:y>0.67703</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -10285,8 +10285,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="8137525" y="3736975"/>
-          <a:ext cx="1752600" cy="390525"/>
+          <a:off x="7780864" y="3800210"/>
+          <a:ext cx="1752956" cy="390794"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -10361,7 +10361,7 @@
         </a:lstStyle>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
-            <a:rPr lang="en-US" sz="1200">
+            <a:rPr lang="en-US" sz="1100">
               <a:solidFill>
                 <a:schemeClr val="bg2">
                   <a:lumMod val="50000"/>
@@ -10371,7 +10371,7 @@
             <a:t>A*</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" sz="1200" baseline="0">
+            <a:rPr lang="en-US" sz="1100" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="bg2">
                   <a:lumMod val="50000"/>
@@ -10380,7 +10380,7 @@
             </a:rPr>
             <a:t> Misplaced Tiles</a:t>
           </a:r>
-          <a:endParaRPr lang="en-US" sz="1200">
+          <a:endParaRPr lang="en-US" sz="1100">
             <a:solidFill>
               <a:schemeClr val="bg2">
                 <a:lumMod val="50000"/>
@@ -11560,8 +11560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C142740-7039-4452-9FA1-0525272298EC}">
   <dimension ref="A1:U11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="Y10" sqref="Y10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11705,19 +11705,19 @@
         <v>2</v>
       </c>
       <c r="M4">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="P4">
         <v>2</v>
       </c>
       <c r="Q4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T4">
         <v>2</v>
       </c>
       <c r="U4">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
@@ -11725,7 +11725,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E5">
         <v>4</v>
@@ -11743,19 +11743,19 @@
         <v>4</v>
       </c>
       <c r="M5">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="P5">
         <v>4</v>
       </c>
       <c r="Q5">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="T5">
         <v>4</v>
       </c>
       <c r="U5">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
@@ -11763,7 +11763,7 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>233</v>
+        <v>309</v>
       </c>
       <c r="E6">
         <v>8</v>
@@ -11781,19 +11781,19 @@
         <v>8</v>
       </c>
       <c r="M6">
-        <v>253</v>
+        <v>188</v>
       </c>
       <c r="P6">
         <v>8</v>
       </c>
       <c r="Q6">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="T6">
         <v>8</v>
       </c>
       <c r="U6">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
@@ -11801,13 +11801,13 @@
         <v>12</v>
       </c>
       <c r="B7">
-        <v>1904</v>
+        <v>2239</v>
       </c>
       <c r="E7">
         <v>12</v>
       </c>
       <c r="F7">
-        <v>96</v>
+        <v>120</v>
       </c>
       <c r="I7">
         <v>12</v>
@@ -11819,19 +11819,19 @@
         <v>12</v>
       </c>
       <c r="M7">
-        <v>2018</v>
+        <v>1268</v>
       </c>
       <c r="P7">
         <v>12</v>
       </c>
       <c r="Q7">
-        <v>113</v>
+        <v>84</v>
       </c>
       <c r="T7">
         <v>12</v>
       </c>
       <c r="U7">
-        <v>50</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
@@ -11839,37 +11839,37 @@
         <v>16</v>
       </c>
       <c r="B8">
-        <v>14570</v>
+        <v>14190</v>
       </c>
       <c r="E8">
         <v>16</v>
       </c>
       <c r="F8">
-        <v>627</v>
+        <v>666</v>
       </c>
       <c r="I8">
         <v>16</v>
       </c>
       <c r="J8">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="L8">
         <v>16</v>
       </c>
       <c r="M8">
-        <v>13429</v>
+        <v>6739</v>
       </c>
       <c r="P8">
         <v>16</v>
       </c>
       <c r="Q8">
-        <v>648</v>
+        <v>414</v>
       </c>
       <c r="T8">
         <v>16</v>
       </c>
       <c r="U8">
-        <v>98</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
@@ -11877,37 +11877,37 @@
         <v>20</v>
       </c>
       <c r="B9">
-        <v>42262</v>
+        <v>41909</v>
       </c>
       <c r="E9">
         <v>20</v>
       </c>
       <c r="F9">
-        <v>2772</v>
+        <v>3146</v>
       </c>
       <c r="I9">
         <v>20</v>
       </c>
       <c r="J9">
-        <v>236</v>
+        <v>503</v>
       </c>
       <c r="L9">
         <v>20</v>
       </c>
       <c r="M9">
-        <v>35026</v>
+        <v>17612</v>
       </c>
       <c r="P9">
         <v>20</v>
       </c>
       <c r="Q9">
-        <v>2892</v>
+        <v>1831</v>
       </c>
       <c r="T9">
         <v>20</v>
       </c>
       <c r="U9">
-        <v>257</v>
+        <v>306</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
@@ -11915,37 +11915,37 @@
         <v>24</v>
       </c>
       <c r="B10">
-        <v>126795</v>
+        <v>134336</v>
       </c>
       <c r="E10">
         <v>24</v>
       </c>
       <c r="F10">
-        <v>14168</v>
+        <v>17769</v>
       </c>
       <c r="I10">
         <v>24</v>
       </c>
       <c r="J10">
-        <v>1391</v>
+        <v>1758</v>
       </c>
       <c r="L10">
         <v>24</v>
       </c>
       <c r="M10">
-        <v>63230</v>
+        <v>24203</v>
       </c>
       <c r="P10">
         <v>24</v>
       </c>
       <c r="Q10">
-        <v>13328</v>
+        <v>8717</v>
       </c>
       <c r="T10">
         <v>24</v>
       </c>
       <c r="U10">
-        <v>1455</v>
+        <v>967</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
@@ -11953,47 +11953,47 @@
         <v>31</v>
       </c>
       <c r="B11">
-        <v>181440</v>
+        <v>181439</v>
       </c>
       <c r="E11">
         <v>31</v>
       </c>
       <c r="F11">
-        <v>122308</v>
+        <v>143849</v>
       </c>
       <c r="I11">
         <v>31</v>
       </c>
       <c r="J11">
-        <v>11877</v>
+        <v>21198</v>
       </c>
       <c r="L11">
         <v>31</v>
       </c>
       <c r="M11">
-        <v>61752</v>
+        <v>25135</v>
       </c>
       <c r="P11">
         <v>31</v>
       </c>
       <c r="Q11">
-        <v>66653</v>
+        <v>25071</v>
       </c>
       <c r="T11">
         <v>31</v>
       </c>
       <c r="U11">
-        <v>12448</v>
+        <v>8862</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="T1:U1"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="L1:M1"/>
     <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="T1:U1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -12004,8 +12004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6395ADF-6F13-4283-83B7-8F134688D095}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T39" sqref="T39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S21" sqref="S21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12171,7 +12171,7 @@
         <v>16</v>
       </c>
       <c r="B8" s="1">
-        <v>120</v>
+        <v>88</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1">
@@ -12193,21 +12193,21 @@
         <v>20</v>
       </c>
       <c r="B9" s="1">
-        <v>424</v>
+        <v>338</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1">
         <v>20</v>
       </c>
       <c r="E9" s="1">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1">
         <v>20</v>
       </c>
       <c r="H9" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -12215,21 +12215,21 @@
         <v>24</v>
       </c>
       <c r="B10" s="1">
-        <v>1518</v>
+        <v>1143</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1">
         <v>24</v>
       </c>
       <c r="E10" s="1">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1">
         <v>24</v>
       </c>
       <c r="H10" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -12237,21 +12237,21 @@
         <v>31</v>
       </c>
       <c r="B11" s="1">
-        <v>2502</v>
+        <v>1540</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1">
         <v>31</v>
       </c>
       <c r="E11" s="1">
-        <v>1531</v>
+        <v>1230</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1">
         <v>31</v>
       </c>
       <c r="H11" s="1">
-        <v>100</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>